<commit_message>
T4.1 re-check temporal scale and resolution
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Uhlmann_Reid.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Uhlmann_Reid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE38DE-3321-432F-BCA3-7B6393424541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8369AE-41AC-4E6D-899B-2E4828E5E8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="609">
   <si>
     <t>Bibliographic Data</t>
   </si>
@@ -4343,7 +4343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4385,7 +4385,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4673,29 +4672,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1450" topLeftCell="A2" activePane="bottomLeft"/>
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-      <selection pane="bottomLeft" activeCell="AI51" sqref="AI51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1455" activePane="bottomLeft"/>
+      <selection activeCell="X14" sqref="X14"/>
+      <selection pane="bottomLeft" activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="18.1796875" customWidth="1"/>
-    <col min="24" max="25" width="32.54296875" customWidth="1"/>
-    <col min="34" max="35" width="17.54296875" customWidth="1"/>
-    <col min="36" max="36" width="18.54296875" customWidth="1"/>
-    <col min="37" max="37" width="19.1796875" customWidth="1"/>
-    <col min="38" max="38" width="17.54296875" customWidth="1"/>
-    <col min="39" max="39" width="14.453125" customWidth="1"/>
-    <col min="40" max="41" width="15.81640625" customWidth="1"/>
-    <col min="42" max="42" width="15.453125" customWidth="1"/>
-    <col min="46" max="46" width="15.1796875" customWidth="1"/>
-    <col min="47" max="47" width="18.54296875" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" customWidth="1"/>
+    <col min="24" max="25" width="32.5703125" customWidth="1"/>
+    <col min="34" max="35" width="17.5703125" customWidth="1"/>
+    <col min="36" max="36" width="18.5703125" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="38" max="38" width="17.5703125" customWidth="1"/>
+    <col min="39" max="39" width="14.42578125" customWidth="1"/>
+    <col min="40" max="41" width="15.85546875" customWidth="1"/>
+    <col min="42" max="42" width="15.42578125" customWidth="1"/>
+    <col min="46" max="46" width="15.140625" customWidth="1"/>
+    <col min="47" max="47" width="18.5703125" customWidth="1"/>
     <col min="48" max="48" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -4761,7 +4760,7 @@
       <c r="AW1" s="13"/>
       <c r="AX1" s="13"/>
     </row>
-    <row r="2" spans="1:51" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:51" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -4913,7 +4912,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -4972,7 +4971,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -5031,7 +5030,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>592</v>
       </c>
@@ -5090,7 +5089,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -5149,7 +5148,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -5209,7 +5208,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -5462,7 +5461,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -5521,7 +5520,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -5640,7 +5639,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -5759,7 +5758,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="13" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:51" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>191</v>
       </c>
@@ -5885,7 +5884,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -5953,10 +5952,7 @@
         <v>168</v>
       </c>
       <c r="X14" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>144</v>
+        <v>267</v>
       </c>
       <c r="Z14" t="s">
         <v>221</v>
@@ -6013,7 +6009,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -6147,7 +6143,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>245</v>
       </c>
@@ -6206,7 +6202,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>256</v>
       </c>
@@ -6328,7 +6324,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>273</v>
       </c>
@@ -6450,7 +6446,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -6575,7 +6571,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>291</v>
       </c>
@@ -6694,7 +6690,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>314</v>
       </c>
@@ -6819,7 +6815,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>328</v>
       </c>
@@ -6950,7 +6946,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>343</v>
       </c>
@@ -7075,7 +7071,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>343</v>
       </c>
@@ -7200,7 +7196,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>357</v>
       </c>
@@ -7328,7 +7324,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>357</v>
       </c>
@@ -7456,7 +7452,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>372</v>
       </c>
@@ -7587,7 +7583,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>387</v>
       </c>
@@ -7718,7 +7714,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>404</v>
       </c>
@@ -7800,7 +7796,7 @@
       <c r="AF29">
         <v>4.3</v>
       </c>
-      <c r="AG29" s="19" t="s">
+      <c r="AG29" t="s">
         <v>497</v>
       </c>
       <c r="AH29" t="s">
@@ -7846,7 +7842,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>415</v>
       </c>
@@ -7971,7 +7967,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>415</v>
       </c>
@@ -8096,7 +8092,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>430</v>
       </c>
@@ -8224,7 +8220,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>442</v>
       </c>
@@ -8352,7 +8348,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="34" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>454</v>
       </c>
@@ -8477,7 +8473,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="35" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>454</v>
       </c>
@@ -8602,7 +8598,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="36" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>454</v>
       </c>
@@ -8721,7 +8717,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="37" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>454</v>
       </c>
@@ -8840,7 +8836,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>465</v>
       </c>
@@ -8968,7 +8964,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>465</v>
       </c>
@@ -9129,20 +9125,20 @@
   <dimension ref="A1:AX38"/>
   <sheetViews>
     <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="32.1796875" customWidth="1"/>
-    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="32" max="32" width="14.54296875" customWidth="1"/>
-    <col min="33" max="33" width="26.453125" customWidth="1"/>
+    <col min="32" max="32" width="14.5703125" customWidth="1"/>
+    <col min="33" max="33" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -9208,7 +9204,7 @@
       <c r="AW1" s="8"/>
       <c r="AX1" s="8"/>
     </row>
-    <row r="2" spans="1:50" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -9360,7 +9356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Q3" t="s">
         <v>69</v>
       </c>
@@ -9417,7 +9413,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="Q4" t="s">
         <v>282</v>
       </c>
@@ -9474,7 +9470,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R5" t="s">
         <v>486</v>
       </c>
@@ -9530,7 +9526,7 @@
       </c>
       <c r="AX5" s="7"/>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>70</v>
       </c>
@@ -9575,7 +9571,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>493</v>
       </c>
@@ -9617,7 +9613,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>499</v>
       </c>
@@ -9655,7 +9651,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>134</v>
       </c>
@@ -9690,7 +9686,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
         <v>236</v>
       </c>
@@ -9725,7 +9721,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
         <v>71</v>
       </c>
@@ -9760,7 +9756,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S12" t="s">
         <v>512</v>
       </c>
@@ -9792,7 +9788,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S13" t="s">
         <v>516</v>
       </c>
@@ -9827,7 +9823,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S14" t="s">
         <v>85</v>
       </c>
@@ -9856,7 +9852,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S15" t="s">
         <v>184</v>
       </c>
@@ -9885,7 +9881,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="S16" t="s">
         <v>527</v>
       </c>
@@ -9905,7 +9901,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="17" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="17" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AM17" t="s">
         <v>189</v>
       </c>
@@ -9913,22 +9909,22 @@
         <v>528</v>
       </c>
     </row>
-    <row r="18" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="18" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ18" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="19" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="19" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ19" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="22" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="22" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH22" s="5" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="23" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="23" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH23" s="6" t="s">
         <v>203</v>
       </c>
@@ -9963,7 +9959,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="24" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="24" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH24" t="s">
         <v>204</v>
       </c>
@@ -9989,7 +9985,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="25" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="25" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH25" t="s">
         <v>536</v>
       </c>
@@ -10012,7 +10008,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="26" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="26" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ26" t="s">
         <v>187</v>
       </c>
@@ -10023,7 +10019,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="27" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="27" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ27" t="s">
         <v>539</v>
       </c>
@@ -10034,7 +10030,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="28" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="28" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AJ28" t="s">
         <v>541</v>
       </c>
@@ -10042,12 +10038,12 @@
         <v>498</v>
       </c>
     </row>
-    <row r="29" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="29" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AQ29" s="5" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="30" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="30" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH30" s="5" t="s">
         <v>542</v>
       </c>
@@ -10070,7 +10066,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="31" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="31" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH31" s="6" t="s">
         <v>204</v>
       </c>
@@ -10096,7 +10092,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="32" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="32" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH32" t="s">
         <v>551</v>
       </c>
@@ -10122,7 +10118,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="33" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="33" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AH33" t="s">
         <v>205</v>
       </c>
@@ -10142,7 +10138,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="34" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="34" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AI34" t="s">
         <v>563</v>
       </c>
@@ -10156,7 +10152,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="35" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="35" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AI35" t="s">
         <v>503</v>
       </c>
@@ -10170,7 +10166,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="36" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="36" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AU36" t="s">
         <v>570</v>
       </c>
@@ -10178,10 +10174,10 @@
         <v>571</v>
       </c>
     </row>
-    <row r="37" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="37" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:48" x14ac:dyDescent="0.35">
+    <row r="38" spans="34:48" x14ac:dyDescent="0.25">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -10209,38 +10205,38 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.54296875" customWidth="1"/>
-    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" customWidth="1"/>
-    <col min="20" max="20" width="19.453125" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" customWidth="1"/>
-    <col min="22" max="22" width="18.54296875" customWidth="1"/>
-    <col min="26" max="26" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.453125" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" customWidth="1"/>
-    <col min="31" max="31" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.81640625" customWidth="1"/>
-    <col min="33" max="33" width="12.54296875" customWidth="1"/>
+    <col min="28" max="28" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" customWidth="1"/>
+    <col min="31" max="31" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -10287,7 +10283,7 @@
       <c r="AF1" s="13"/>
       <c r="AG1" s="13"/>
     </row>
-    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -10388,7 +10384,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>477</v>
       </c>
@@ -10454,7 +10450,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>481</v>
       </c>
@@ -10505,7 +10501,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>486</v>
       </c>
@@ -10559,7 +10555,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -10601,7 +10597,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>493</v>
       </c>
@@ -10646,7 +10642,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>499</v>
       </c>
@@ -10684,7 +10680,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -10722,7 +10718,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>236</v>
       </c>
@@ -10757,7 +10753,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>71</v>
       </c>
@@ -10789,7 +10785,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>512</v>
       </c>
@@ -10821,7 +10817,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>516</v>
       </c>
@@ -10850,7 +10846,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>85</v>
       </c>
@@ -10873,7 +10869,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>184</v>
       </c>
@@ -10899,7 +10895,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>527</v>
       </c>
@@ -10916,7 +10912,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="17" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
         <v>223</v>
       </c>
@@ -10927,7 +10923,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="18" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q18" t="s">
         <v>92</v>
       </c>
@@ -10941,7 +10937,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="19" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R19" t="s">
         <v>546</v>
       </c>
@@ -10955,7 +10951,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="20" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S20" t="s">
         <v>558</v>
       </c>
@@ -10966,7 +10962,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="21" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S21" t="s">
         <v>576</v>
       </c>
@@ -10980,7 +10976,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="22" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S22" t="s">
         <v>503</v>
       </c>
@@ -10991,7 +10987,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="23" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q23" t="s">
         <v>531</v>
       </c>
@@ -11002,7 +10998,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="24" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R24" t="s">
         <v>484</v>
       </c>
@@ -11010,7 +11006,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="25" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R25" t="s">
         <v>488</v>
       </c>
@@ -11018,7 +11014,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="26" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R26" t="s">
         <v>190</v>
       </c>
@@ -11026,7 +11022,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="27" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R27" t="s">
         <v>498</v>
       </c>
@@ -11040,7 +11036,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="28" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q28" t="s">
         <v>518</v>
       </c>
@@ -11051,7 +11047,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="29" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R29" t="s">
         <v>537</v>
       </c>
@@ -11062,7 +11058,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="30" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q30" t="s">
         <v>522</v>
       </c>
@@ -11073,7 +11069,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="31" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R31" t="s">
         <v>538</v>
       </c>
@@ -11081,7 +11077,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="32" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
         <v>532</v>
       </c>
@@ -11089,12 +11085,12 @@
         <v>503</v>
       </c>
     </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z34" t="s">
         <v>498</v>
       </c>
@@ -11114,12 +11110,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11237,15 +11230,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11267,16 +11270,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>